<commit_message>
Updated docker stack to include a jupyter notebook server.
</commit_message>
<xml_diff>
--- a/jupyter_demos/review_extractor/reviews.xlsx
+++ b/jupyter_demos/review_extractor/reviews.xlsx
@@ -505,12 +505,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>customer service issues</t>
+          <t>delayed delivery</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -518,12 +518,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/users/62bf16a05eb62f0012184c27</t>
+          <t>/users/6687117c86aa70596d703aaf</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ash</t>
+          <t>Mr. James Opoku</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -533,23 +533,18 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Absolute cowboys</t>
+          <t>I applied for a credit card and was…</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Absolute cowboys, customer help desk is a joke if you get through, try to rip you off as much as they can . I tried to close my account ( which they make increasingly difficult ) the person on the end of the phone had no idea and was trying to tell me I owed more than I did and when I questioned it they put it down to computer error !!!! Tried to complain to the complaints department and got standard can’t help you apology 
-</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Reply from  118 118 MONEY
-Hello Ash - thanks for leaving a review. I'm sorry to hear that you're not happy. I have sent you a request for more information. If you'd like, I can arrange for a member of the team to contact you to discuss this. Kind regards, Sam Customer Engagement team.</t>
-        </is>
-      </c>
+          <t xml:space="preserve">I applied for a credit card and was notified that it had been dispatched. About 2 weeks down the line and I’ve still not received it
+</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" s="2" t="n">
-        <v>45476</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="3">
@@ -563,7 +558,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>company takes advantage, bad customer service</t>
+          <t>customer service is bad</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -576,12 +571,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/users/64ef4382cb6b190012a45b84</t>
+          <t>/users/62bf16a05eb62f0012184c27</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Mathew Thomas</t>
+          <t>Ash</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -591,19 +586,19 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Awful company</t>
+          <t>Absolute cowboys</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Awful company, believe me once they have your bank details they will help themselves to whatever they want whenever they want.Customer service are useless and the complaints team are less than useless and will just send standard responses very close to the contracted deadlines.Do yourselves a favour and visit a loan shark instead of this cowboy outfit as the service you receive will be more compassionate.Escalating complaint to FOS
+          <t xml:space="preserve">Absolute cowboys, customer help desk is a joke if you get through, try to rip you off as much as they can . I tried to close my account ( which they make increasingly difficult ) the person on the end of the phone had no idea and was trying to tell me I owed more than I did and when I questioned it they put it down to computer error !!!! Tried to complain to the complaints department and got standard can’t help you apology 
 </t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Matthew - I'm sorry to hear about your frustrations. I can see that you've been in discussion with our Complaints team about this. If you would like to discuss the response we've sent to you, please do get back in touch. We have explained that we will only collect payments from you, in line with the T&amp;Cs of your contract, and only when due.Kind regards, Sam Customer Engagement team.</t>
+Hello Ash - thanks for leaving a review. I'm sorry to hear that you're not happy. I have sent you a request for more information. If you'd like, I can arrange for a member of the team to contact you to discuss this. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L3" s="2" t="n">
@@ -621,7 +616,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ruined credit score due to genuine mistake</t>
+          <t>untrustworthy and poor customer service</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -634,12 +629,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>/users/66853451836f3a5f8cd9365b</t>
+          <t>/users/64ef4382cb6b190012a45b84</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Jasper Libby</t>
+          <t>Mathew Thomas</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -649,18 +644,23 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">NEVER USE </t>
+          <t>Awful company</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Absolutely awful experience with 118.Paid off my credit card with never missing a payment.I paid off my credit card so the balance on the card was £0.They then charged my subscription fee of £8 which I didnt notice, me being me didn't realise they still charged this fee after you paid the card off. So I hold my hands up to that.Logged onto my online app on the Monday when the payment was due and thought I paid for the £8 there and then for this subscription fee but for some reason it didnt go through, no idea why.118 contacted me on the Tuesday saying payment missed, and this will now effect my credit.But this is a subscription fee? The card isnt in arreas, the balance is £0 why should they classed this as missed payment? Anyway, seeing as I was a day late in paying for the subscription fee even though the card was at £0 they put this down as a missed payment which will now go down on my credit report, which will now effect all my future plans with buying my first home. Tried to call 118 to beg them this was a genuine mistake but they said they couldn't do anything about it, and couldn't change the fact that even though I was just 12 hours "late" in not paying back the subscription fee it was going as a missed payment, and I would need to contact all the credit agencies to dispute this... which we all know is an absolute nightmare. They were no help what so ever and they didn't even take into account how much this will financially ruin me. I've worked so hard to get my credit score up to excellent and due to this genuine mistake they have ruined it all for me. Also tried to close my account and they finally closed it after the third request.An absolute awful company who really will do nothing for you. I was so upset on the phone and the lady was so robotic SO textbook.Didnt take into my personal situation at all, and the whole company are so heartless and just disgusting. 
-</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+          <t xml:space="preserve">Awful company, believe me once they have your bank details they will help themselves to whatever they want whenever they want.Customer service are useless and the complaints team are less than useless and will just send standard responses very close to the contracted deadlines.Do yourselves a favour and visit a loan shark instead of this cowboy outfit as the service you receive will be more compassionate.Escalating complaint to FOS
+</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Reply from  118 118 MONEY
+Hello Matthew - I'm sorry to hear about your frustrations. I can see that you've been in discussion with our Complaints team about this. If you would like to discuss the response we've sent to you, please do get back in touch. We have explained that we will only collect payments from you, in line with the T&amp;Cs of your contract, and only when due.Kind regards, Sam Customer Engagement team.</t>
+        </is>
+      </c>
       <c r="L4" s="2" t="n">
-        <v>45475</v>
+        <v>45476</v>
       </c>
     </row>
     <row r="5">
@@ -674,7 +674,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>unreliable app, no customer service</t>
+          <t>ruined credit score due to genuine mistake</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -687,12 +687,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>/users/5b9aef214de5666d34b34f4e</t>
+          <t>/users/66853451836f3a5f8cd9365b</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tom Obemiaso</t>
+          <t>Jasper Libby</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -702,23 +702,23 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stay clear of 118 money </t>
+          <t xml:space="preserve">NEVER USE </t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stay clear of 118 money , credit cards or loans. The company is so bad ..  the app is unreliable, you are never able to get customer service on the phone and the interest rates ... they are comparable to loan sharks. How this company is still in business is a failing of the financial ombudsman.
+          <t xml:space="preserve">Absolutely awful experience with 118.Paid off my credit card with never missing a payment.I paid off my credit card so the balance on the card was £0.They then charged my subscription fee of £8 which I didnt notice, me being me didn't realise they still charged this fee after you paid the card off. So I hold my hands up to that.Logged onto my online app on the Monday when the payment was due and thought I paid for the £8 there and then for this subscription fee but for some reason it didnt go through, no idea why.118 contacted me on the Tuesday saying payment missed, and this will now effect my credit.But this is a subscription fee? The card isnt in arreas, the balance is £0 why should they classed this as missed payment? Anyway, seeing as I was a day late in paying for the subscription fee even though the card was at £0 they put this down as a missed payment which will now go down on my credit report, which will now effect all my future plans with buying my first home. Tried to call 118 to beg them this was a genuine mistake but they said they couldn't do anything about it, and couldn't change the fact that even though I was just 12 hours "late" in not paying back the subscription fee it was going as a missed payment, and I would need to contact all the credit agencies to dispute this... which we all know is an absolute nightmare. They were no help what so ever and they didn't even take into account how much this will financially ruin me. I've worked so hard to get my credit score up to excellent and due to this genuine mistake they have ruined it all for me. Also tried to close my account and they finally closed it after the third request.An absolute awful company who really will do nothing for you. I was so upset on the phone and the lady was so robotic SO textbook.Didnt take into my personal situation at all, and the whole company are so heartless and just disgusting. 
 </t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Tom, thank you for leaving a review. I'm sorry to hear that you're frustrated with the app and that you've had trouble getting hold of us on the phone. Please respond to the information request I've sent - I'd like to arrange for a member of the Customer Support team to contact you. Kind regards, Sam Customer Engagement team.</t>
+Hi Jasper, thanks for the review.We’re sorry to hear that you’ve been unhappy with our service.A subscription fee forms part of your payment/balance. As the card is a subscription-based card, this means you’d be charged the subscription fee, regardless of the balance being £0, or at its max. This would be confirmed in your documentation, which you confirm that you’ve read and understood by signing said documentation.As the subscription fee forms part of the payment/balance, if this isn’t paid, then it’s classed as a late/missed payment. We have an obligation to provide a true and accurate representation of how an account is maintained with us, to the Credit Reference Agencies (CRA’s). We’re sorry that you feel we’re unwilling to help you. Please keep in mind that we’re not able to falsely report to your credit file.If you’d like to express your concerns further, you can reach out to our Complaints team through our online feedback/complaints form found on our website. LM</t>
         </is>
       </c>
       <c r="L5" s="2" t="n">
-        <v>45474</v>
+        <v>45475</v>
       </c>
     </row>
     <row r="6">
@@ -732,12 +732,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>aggressive collection practices</t>
+          <t>unreliable app, poor customer service</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>customer service, speed</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -745,12 +745,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>/users/5ef3474ad9f9fa305970a609</t>
+          <t>/users/5b9aef214de5666d34b34f4e</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>David Holmes</t>
+          <t>Tom Obemiaso</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -760,19 +760,19 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Really poor</t>
+          <t xml:space="preserve">Stay clear of 118 money </t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Really poor, you miss a payment and the next day there are phone call after phone call chasing you. It’s so aggressive too early on from missing it and what I don’t like is that the number is disguised as a mobile phone number making it look like a friend not a business 
+          <t xml:space="preserve">Stay clear of 118 money , credit cards or loans. The company is so bad ..  the app is unreliable, you are never able to get customer service on the phone and the interest rates ... they are comparable to loan sharks. How this company is still in business is a failing of the financial ombudsman.
 </t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello David, Thank you for leaving a review. When a customer misses a payment, it can have a detrimental impact on their credit score. So, when contacting customers who have fallen behind with payments, it's our intention to help. Note that the number we call from ends 118 and we send a follow up SMS to confirm it was us calling. Thank you for replying to my information request. I've asked a member of the Customer Support team to contact you.Kind regards, Sam Customer Engagement team.</t>
+Hello Tom, thank you for leaving a review. I'm sorry to hear that you're frustrated with the app and that you've had trouble getting hold of us on the phone. Please respond to the information request I've sent - I'd like to arrange for a member of the Customer Support team to contact you. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L6" s="2" t="n">
@@ -790,12 +790,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>site problem</t>
+          <t>aggressive debt chasing</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>website issues</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -803,12 +803,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>/users/6683a648078852695571de22</t>
+          <t>/users/5ef3474ad9f9fa305970a609</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Mr. Kevin Mattammal Jacob</t>
+          <t>David Holmes</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -818,23 +818,23 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>i didn't get the credit card site…</t>
+          <t>Really poor</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">i didn't get the credit card site problem
+          <t xml:space="preserve">Really poor, you miss a payment and the next day there are phone call after phone call chasing you. It’s so aggressive too early on from missing it and what I don’t like is that the number is disguised as a mobile phone number making it look like a friend not a business 
 </t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Kevin - thank you for leaving a review and letting us know. A member of the Customer Support team will contact you this morning to get this resolved for you.Kind regards Sam Customer Engagement team.</t>
+Hello David, Thank you for leaving a review. When a customer misses a payment, it can have a detrimental impact on their credit score. So, when contacting customers who have fallen behind with payments, it's our intention to help. Note that the number we call from ends 118 and we send a follow up SMS to confirm it was us calling. Thank you for replying to my information request. I've asked a member of the Customer Support team to contact you.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L7" s="2" t="n">
-        <v>45475</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="8">
@@ -848,25 +848,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>poor service</t>
+          <t>credit card site problem</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>customer service</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
+          <t>website issues</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>/users/6678539275540f736b963287</t>
+          <t>/users/6683a648078852695571de22</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Mrs. Udaya Kuntamukkala</t>
+          <t>Mr. Kevin Mattammal Jacob</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -876,23 +874,23 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Poor</t>
+          <t>i didn't get the credit card site…</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poor and worst
+          <t xml:space="preserve">i didn't get the credit card site problem
 </t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - I'm sorry to hear you're not happy. We would like to investigate and respond to any feedback you have for us. I have asked a member of our Customer Support team to reach out to you. Alternatively, you can email us at complaints@118118money.com.Kind regards, SamCustomer Engagement team</t>
+Hi Kevin - thank you for leaving a review and letting us know. A member of the Customer Support team will contact you this morning to get this resolved for you.Kind regards Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L8" s="2" t="n">
-        <v>45466</v>
+        <v>45475</v>
       </c>
     </row>
     <row r="9">
@@ -906,12 +904,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>company cancelled loan agreement without discussion</t>
+          <t>poor service</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -919,12 +917,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>/users/6676f73cd305a1f3d139191c</t>
+          <t>/users/6678539275540f736b963287</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Fred</t>
+          <t>Mrs. Udaya Kuntamukkala</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -934,23 +932,23 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Loan agreement</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Had a payment plan put in place for  three months as struggling, following this full payments would resume at full amount. they cancelled loan agreement after three months and reduced payments further without any discussions and report negatively on credit report. Please stay clear of this company
+          <t xml:space="preserve">Poor and worst
 </t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - thank you for leaving a review. I have sent a request for more information so that we can look into this for you. Alternatively, please send an email to complaints@118118money.com.Kind regards Sam Customer Engagement team.</t>
+Hello - I'm sorry to hear you're not happy. We would like to investigate and respond to any feedback you have for us. I have asked a member of our Customer Support team to reach out to you. Alternatively, you can email us at complaints@118118money.com.Kind regards, SamCustomer Engagement team</t>
         </is>
       </c>
       <c r="L9" s="2" t="n">
-        <v>45465</v>
+        <v>45466</v>
       </c>
     </row>
     <row r="10">
@@ -964,7 +962,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>unauthorized payments and poor customer service</t>
+          <t>unfair treatment by lender</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -977,12 +975,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>/users/5fd46788ed74d7001a4b3dbc</t>
+          <t>/users/6676f73cd305a1f3d139191c</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Andy Jaszczyk</t>
+          <t>Fred</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -992,19 +990,19 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>The worst company I have ever know</t>
+          <t>Loan agreement</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">The worst company I have ever know. They take money out of your account with out your permission just because it’s been used to make a payment once. After they have told them to take the account off the system they then take a payment again so clearly haven’t. When you call to speak to someone they aren’t helpful. They give you different values that you owe as a payment. After taking money out of an account they don’t have authorisation on, say you owe the amount again then when you pay that money still hound you with multiple calls per day. When you speak to them they say “every manager is a meeting” they then end your call. Even worse communication and telephone manor than British Gas and that’s saying something. Everyone avoid at all costs 
+          <t xml:space="preserve">Had a payment plan put in place for  three months as struggling, following this full payments would resume at full amount. they cancelled loan agreement after three months and reduced payments further without any discussions and report negatively on credit report. Please stay clear of this company
 </t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Alternatively, please email complaints@118118money.com.Kind regards,Sam</t>
+Hello - thank you for leaving a review. I have sent a request for more information so that we can look into this for you. Alternatively, please send an email to complaints@118118money.com.Kind regards Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L10" s="2" t="n">
@@ -1022,7 +1020,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>unhelpful and unfair customer service</t>
+          <t>unauthorized payments and poor customer service</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1035,12 +1033,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>/users/5dab8bc2e5189914ae8677e3</t>
+          <t>/users/5fd46788ed74d7001a4b3dbc</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Sandra R.</t>
+          <t>Andy Jaszczyk</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1050,23 +1048,23 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Awful and unhelpful</t>
+          <t>The worst company I have ever know</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t xml:space="preserve">I have tried on several occasions to request refunds from 118 118 for transactions that I had processed. One had been a show I attended which went really badly, was chaotic and awful. I had contacted the organisers of the event asking for my refund and because they are based outside the country, they declined refund. Naturally I went to my credit card company (118) who refused to refund the money stating “you attended the event, it wasn’t cancelled” and declined to help me further.Second time I made a payment for a holiday thinking I was paying for a deposit only to realise a full payment was taken from my card. Within 12hrs of getting the notification I contacted 118 asking them to reverse the payment. I was told we can’t because it’s still showing as pending. When it was cleared I rang 118 begging them to cancel the payment as it was a genuine mistake. I was I told we don’t do that because the company did not cancel the holiday. What is the point of having a credit card? This company is very very unhelpful and extremely unfair. After finishing my payment I will be cancelling my credit card account. 
+          <t xml:space="preserve">The worst company I have ever know. They take money out of your account with out your permission just because it’s been used to make a payment once. After they have told them to take the account off the system they then take a payment again so clearly haven’t. When you call to speak to someone they aren’t helpful. They give you different values that you owe as a payment. After taking money out of an account they don’t have authorisation on, say you owe the amount again then when you pay that money still hound you with multiple calls per day. When you speak to them they say “every manager is a meeting” they then end your call. Even worse communication and telephone manor than British Gas and that’s saying something. Everyone avoid at all costs 
 </t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - I have sent a request for more information to be able to identify your account. If you can provide your contact details, I can arrange for a member of our Customer Support team to contact you. Alternatively, you can e-mail us: complaints@118118money.com.Kind regards, Sam Customer Engagement team.</t>
+I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Alternatively, please email complaints@118118money.com.Kind regards,Sam</t>
         </is>
       </c>
       <c r="L11" s="2" t="n">
-        <v>45457</v>
+        <v>45465</v>
       </c>
     </row>
     <row r="12">
@@ -1080,12 +1078,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>never received card</t>
+          <t>unhelpful and unfair customer service</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -1093,12 +1091,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>/users/667143945a651fda859931b5</t>
+          <t>/users/5dab8bc2e5189914ae8677e3</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Miss. Diana Brown</t>
+          <t>Sandra R.</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1108,23 +1106,23 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Never received my card</t>
+          <t>Awful and unhelpful</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Never received my card 
+          <t xml:space="preserve">I have tried on several occasions to request refunds from 118 118 for transactions that I had processed. One had been a show I attended which went really badly, was chaotic and awful. I had contacted the organisers of the event asking for my refund and because they are based outside the country, they declined refund. Naturally I went to my credit card company (118) who refused to refund the money stating “you attended the event, it wasn’t cancelled” and declined to help me further.Second time I made a payment for a holiday thinking I was paying for a deposit only to realise a full payment was taken from my card. Within 12hrs of getting the notification I contacted 118 asking them to reverse the payment. I was told we can’t because it’s still showing as pending. When it was cleared I rang 118 begging them to cancel the payment as it was a genuine mistake. I was I told we don’t do that because the company did not cancel the holiday. What is the point of having a credit card? This company is very very unhelpful and extremely unfair. After finishing my payment I will be cancelling my credit card account. 
 </t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - please accept our aplogies for the delay in responding to your review. I have asked a member of our Customer Support team to contact you, to make sure everything is now okay and you have recieved your card.Kind regards,Sam Customer Engagement team.</t>
+Hello - I have sent a request for more information to be able to identify your account. If you can provide your contact details, I can arrange for a member of our Customer Support team to contact you. Alternatively, you can e-mail us: complaints@118118money.com.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L12" s="2" t="n">
-        <v>45446</v>
+        <v>45457</v>
       </c>
     </row>
     <row r="13">
@@ -1138,12 +1136,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>terrible customer service</t>
+          <t>never received card</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -1151,12 +1149,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>/users/6670161c05db3126999e44f4</t>
+          <t>/users/667143945a651fda859931b5</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Rebecca Howard</t>
+          <t>Miss. Diana Brown</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1166,23 +1164,23 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Absolutely disgraceful treatment of…</t>
+          <t>Never received my card</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Absolutely disgraceful treatment of their customers struggling to pay one payment. I am currently in Australia having relocated and as such, have changed jobs and have unfortunately not been able to pay last months payment. I proactively emailed the customer service email address to tell them about this and advise I would make double payment this month.  I have received daily emails from a no reply address and texts from a no reply number demanding I pay or they will take legal action. I have emailed multiple times to the only email address I can find on the internet. I can’t access their website as they block IPs outside of UK and I cannot download the app as it’s only available on the UK App Store. What am I meant to do?! Terrible customer service. All I have asked for is your bank details so I can pay the outstanding monthly amount, and I am being bombarded by automated abuse. 
+          <t xml:space="preserve">Never received my card 
 </t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Rebecca, I am sorry to hear about your frustrations. Thank you for leaving a review. I have sent a request for more information - please provide your contact details (doing so is private) and I will arrange for a member of the team to contact you as soon as possible.Kind regards SamCustomer Engagement team.</t>
+Hello - please accept our aplogies for the delay in responding to your review. I have asked a member of our Customer Support team to contact you, to make sure everything is now okay and you have recieved your card.Kind regards,Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L13" s="2" t="n">
-        <v>45460</v>
+        <v>45446</v>
       </c>
     </row>
     <row r="14">
@@ -1196,12 +1194,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>can't access account on holiday</t>
+          <t>unacceptable treatment and poor customer service</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>account access</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1209,12 +1207,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>/users/661aaf72912cf30012412fb8</t>
+          <t>/users/6670161c05db3126999e44f4</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Katy</t>
+          <t>Rebecca Howard</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1224,23 +1222,23 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Wouldn't let me go on my account whilst…</t>
+          <t>Absolutely disgraceful treatment of…</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Wouldn't let me go on my account whilst I'm on holiday, ignored my emails but still keep sending me arrears emails.. why don't you sort it out so people can get on the website or app when they are on holiday. What happens if my card gets stolen.. do I just wait until I get home?Update: After a complaint was raised, again 118 closed it stating I had never emailed them. So I replied with the evidence (screenshot of my sent emails) and then they started ignoring me again. I find that they try and avoid you when you are right and can prove it, they would of seen my sent emails so clearly they lied. 
+          <t xml:space="preserve">Absolutely disgraceful treatment of their customers struggling to pay one payment. I am currently in Australia having relocated and as such, have changed jobs and have unfortunately not been able to pay last months payment. I proactively emailed the customer service email address to tell them about this and advise I would make double payment this month.  I have received daily emails from a no reply address and texts from a no reply number demanding I pay or they will take legal action. I have emailed multiple times to the only email address I can find on the internet. I can’t access their website as they block IPs outside of UK and I cannot download the app as it’s only available on the UK App Store. What am I meant to do?! Terrible customer service. All I have asked for is your bank details so I can pay the outstanding monthly amount, and I am being bombarded by automated abuse. 
 </t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Katy - thank you for leaving a review. I have noted and will raise your feedback. I'm sorry to hear of your frustrations. I have sent you a request for more information - if you still need to speak to us, please respond to that and I will arrange for a member of the Customer Support team to contact you as soon as possible.Kind regardsSam Customer Engagement team.</t>
+Hello Rebecca, I am sorry to hear about your frustrations. Thank you for leaving a review. I have sent a request for more information - please provide your contact details (doing so is private) and I will arrange for a member of the team to contact you as soon as possible.Kind regards SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L14" s="2" t="n">
-        <v>45458</v>
+        <v>45460</v>
       </c>
     </row>
     <row r="15">
@@ -1254,12 +1252,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>high fees</t>
+          <t>account access issues on holiday</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>high price/interest rate</t>
+          <t>issues on holiday</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1267,12 +1265,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>/users/542433ac00006400018c88ec</t>
+          <t>/users/661aaf72912cf30012412fb8</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Andy Rout</t>
+          <t>Katy</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1282,23 +1280,23 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>owed 8.50  1 month of 55 telephone…</t>
+          <t>Wouldn't let me go on my account whilst…</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t xml:space="preserve">owed 8.50  1 month of 55 telephone calls 48 texts and 50 emails. they must be desperate for cash
+          <t xml:space="preserve">Wouldn't let me go on my account whilst I'm on holiday, ignored my emails but still keep sending me arrears emails.. why don't you sort it out so people can get on the website or app when they are on holiday. What happens if my card gets stolen.. do I just wait until I get home?Update: After a complaint was raised, again 118 closed it stating I had never emailed them. So I replied with the evidence (screenshot of my sent emails) and then they started ignoring me again. I find that they try and avoid you when you are right and can prove it, they would of seen my sent emails so clearly they lied. 
 </t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Andy, thanks for leaving a review. In circumstances where payments are overdue, it is important that we speak to you to try and resolve the situation, as being in arrears can have a negative impact on your credit file. It's our aim to help and support customers if they are struggling. Kind regards, Sam Customer Engagement team.</t>
+Hello Katy - thank you for leaving a review. I have noted and will raise your feedback. I'm sorry to hear of your frustrations. I have sent you a request for more information - if you still need to speak to us, please respond to that and I will arrange for a member of the Customer Support team to contact you as soon as possible.Kind regardsSam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L15" s="2" t="n">
-        <v>45457</v>
+        <v>45458</v>
       </c>
     </row>
     <row r="16">
@@ -1312,12 +1310,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>dislike with service/website</t>
+          <t>high phone bill</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>issues on website</t>
+          <t>price/interest rate</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1325,12 +1323,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>/users/5a85df2df675864e5602c84a</t>
+          <t>/users/542433ac00006400018c88ec</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Darran Watson</t>
+          <t>Andy Rout</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1340,23 +1338,23 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>What a total faff</t>
+          <t>owed 8.50  1 month of 55 telephone…</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t xml:space="preserve">What a total faff, log on to this code, oh yeah total crap, load of bull, will be returning card as soon as it arrives, just as the Zopla card, pennies limit… keep it… Do not use 118 money…
+          <t xml:space="preserve">owed 8.50  1 month of 55 telephone calls 48 texts and 50 emails. they must be desperate for cash
 </t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Darran - I would like to try and understand your frustrations so that we can help. I have asked a member of our Customer Support team to contact you. Kind regards, Sam Customer Engagement team.</t>
+Hi Andy, thanks for leaving a review. In circumstances where payments are overdue, it is important that we speak to you to try and resolve the situation, as being in arrears can have a negative impact on your credit file. It's our aim to help and support customers if they are struggling. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L16" s="2" t="n">
-        <v>45456</v>
+        <v>45457</v>
       </c>
     </row>
     <row r="17">
@@ -1370,12 +1368,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>poor customer service experience</t>
+          <t>returns and credit limits</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>account access</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1383,12 +1381,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>/users/666860f7241bd923355039b0</t>
+          <t>/users/5a85df2df675864e5602c84a</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Matthew John Barrow</t>
+          <t>Darran Watson</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1398,23 +1396,23 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Really bad customer service &amp;…</t>
+          <t>What a total faff</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Really bad customer service &amp; experience.I have a good credit history and credit score - Experian and Equifax are happy that I have the all the particulars I need, but 118118 declined right at the last moment for a reason they don't even know and can not explain.When I asked to speak with someone that can help me understand that decision - because it makes no sense whatsoever - the customer service representative (if that's what you want to call it) told me that there was no one to speak with and hung up on me.There are many many service providers out there with a better understanding of their own business and the ethical requirements as a service provider - Use them instead!
+          <t xml:space="preserve">What a total faff, log on to this code, oh yeah total crap, load of bull, will be returning card as soon as it arrives, just as the Zopla card, pennies limit… keep it… Do not use 118 money…
 </t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Matthew - I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Alternatively, please email complaints@118118money.com.Kind regards, Sam Customer Engagement team.</t>
+Hi Darran - I would like to try and understand your frustrations so that we can help. I have asked a member of our Customer Support team to contact you. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L17" s="2" t="n">
-        <v>45454</v>
+        <v>45456</v>
       </c>
     </row>
     <row r="18">
@@ -1428,7 +1426,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>credit score severely affected by company's inaction</t>
+          <t>bad customer experience</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1441,12 +1439,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>/users/66685f6ec485c04a8e1e4b0e</t>
+          <t>/users/666860f7241bd923355039b0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Consumer</t>
+          <t>Matthew John Barrow</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1456,19 +1454,19 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stay well away from this company </t>
+          <t>Really bad customer service &amp;…</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Absolute disgrace of a company I have had to contact the financial ombudsman over this company various emails just ignored complaint ignored twice via email my credit score was severely affected due to 118 118 money ignoring what needed to be amended on my credit file now I have to wait a further 90 days to get this amended I have now logged this with there ceo he is the only one in the company who has responded I’m now waiting a further reply from the head of customer services I won’t hold my breath I will be instructing solicitors if you email the complaints team they ignore you 
+          <t xml:space="preserve">Really bad customer service &amp; experience.I have a good credit history and credit score - Experian and Equifax are happy that I have the all the particulars I need, but 118118 declined right at the last moment for a reason they don't even know and can not explain.When I asked to speak with someone that can help me understand that decision - because it makes no sense whatsoever - the customer service representative (if that's what you want to call it) told me that there was no one to speak with and hung up on me.There are many many service providers out there with a better understanding of their own business and the ethical requirements as a service provider - Use them instead!
 </t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Kind regards,Sam</t>
+Hello Matthew - I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Alternatively, please email complaints@118118money.com.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L18" s="2" t="n">
@@ -1486,12 +1484,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>declined despite providing all necessary info</t>
+          <t>company ignored emails and complaint</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1499,12 +1497,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>/users/5def98b11ef7dc14c0dc99ec</t>
+          <t>/users/66685f6ec485c04a8e1e4b0e</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Consumer</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1514,23 +1512,23 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>I was accepted for a loan of 2500…</t>
+          <t xml:space="preserve">Stay well away from this company </t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t xml:space="preserve">I was accepted for a loan of 2500 pounds over 3 years. Signed the forms gave them my bank details and card details as i was told id been approved. Gave them all the information they requested to be then told declined. Shocking service and system in place as they also done hard credit check which is now on my file. I want this removed as i didnt recieve the product after a hard credit check. 
+          <t xml:space="preserve">Absolute disgrace of a company I have had to contact the financial ombudsman over this company various emails just ignored complaint ignored twice via email my credit score was severely affected due to 118 118 money ignoring what needed to be amended on my credit file now I have to wait a further 90 days to get this amended I have now logged this with there ceo he is the only one in the company who has responded I’m now waiting a further reply from the head of customer services I won’t hold my breath I will be instructing solicitors if you email the complaints team they ignore you 
 </t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Jei, thanks for the review.We're sorry to hear that you've been unhappy with our service.With any pre-approved offer, the offer is subject to full and final verification/checks; this should be confirmed before submitting the full application.Should you wish to raise your concerns as a complaint; please reach out to our Complaints team through our online complaint/feedback form found on our website.LM</t>
+I am sorry to hear of your frustrations and thank you for leaving a review. I have sent you a request for more information. Please reply to this so we can investigate your comments and arrange for a member of the team to contact you. Kind regards,Sam</t>
         </is>
       </c>
       <c r="L19" s="2" t="n">
-        <v>45450</v>
+        <v>45454</v>
       </c>
     </row>
     <row r="20">
@@ -1544,12 +1542,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>quote not provided, settlement issues</t>
+          <t>declined without receiving loan</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>credit search problems</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1557,12 +1555,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>/users/5cfa999c99e2184536d1f6db</t>
+          <t>/users/5def98b11ef7dc14c0dc99ec</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Ertu Muslu</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1572,23 +1570,23 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>They won't let you settle your loan</t>
+          <t>I was accepted for a loan of 2500…</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t xml:space="preserve">I had a loan with them in a desperate situation for very short term. When I wanted to settle the loan within a month they kept telling me they would send me the quote but no one sent me anything. The app doesn't work and keeps taking monthly money. 
+          <t xml:space="preserve">I was accepted for a loan of 2500 pounds over 3 years. Signed the forms gave them my bank details and card details as i was told id been approved. Gave them all the information they requested to be then told declined. Shocking service and system in place as they also done hard credit check which is now on my file. I want this removed as i didnt recieve the product after a hard credit check. 
 </t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Ertu, thanks for the review.We're sorry to hear that you've been unhappy with our service. We sent you a request for further information in order for us to investigate further; however we've not received a reply.Based on the limited information to hand, we've been unable to match your review to an account; therefore we cannot be any more specific for you at this time. Should you wish to raise your concerns further, please reach out to our Complaints team through our online complaint/feedback form found on our website.LM</t>
+Hi Jei, thanks for the review.We're sorry to hear that you've been unhappy with our service.With any pre-approved offer, the offer is subject to full and final verification/checks; this should be confirmed before submitting the full application.Should you wish to raise your concerns as a complaint; please reach out to our Complaints team through our online complaint/feedback form found on our website.LM</t>
         </is>
       </c>
       <c r="L20" s="2" t="n">
-        <v>45447</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="21">
@@ -1602,12 +1600,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Refund not handled quickly or understandingly</t>
+          <t>quote not provided</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1615,12 +1613,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>/users/5db1f7d2a36427601bc23fc1</t>
+          <t>/users/5cfa999c99e2184536d1f6db</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Matthew Gaughran</t>
+          <t>Ertu Muslu</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1630,23 +1628,23 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Disgraceful </t>
+          <t>They won't let you settle your loan</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Really unhappy. Loan ended and they still took a full payment! Had to contact them myself. Waited ages to speak to someone who struggled to understand me, there was a clear language barrier. The refund for the overpayment isn't instant and I have to wait for it. The advisor wasn't understanding or compassionate regarding the clear issue. Raised a complaint to be advised they have over 4 weeks to respond. Disgusting Update:A complaint was only raised today. Even though I asked the agent on the day to raise a complaint. Joke of a company.
+          <t xml:space="preserve">I had a loan with them in a desperate situation for very short term. When I wanted to settle the loan within a month they kept telling me they would send me the quote but no one sent me anything. The app doesn't work and keeps taking monthly money. 
 </t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Matthew, thanks for the review.We're sorry to hear of the issues you've faced. We can see that a complaint has been raised and our Complaints team will be in touch in due course regarding your concerns.We can see that the payment was refunded the same day for you.LM</t>
+Hi Ertu, thanks for the review.We're sorry to hear that you've been unhappy with our service. We sent you a request for further information in order for us to investigate further; however we've not received a reply.Based on the limited information to hand, we've been unable to match your review to an account; therefore we cannot be any more specific for you at this time. Should you wish to raise your concerns further, please reach out to our Complaints team through our online complaint/feedback form found on our website.LM</t>
         </is>
       </c>
       <c r="L21" s="2" t="n">
-        <v>45446</v>
+        <v>45447</v>
       </c>
     </row>
     <row r="22">
@@ -1660,7 +1658,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>bad customer service</t>
+          <t>late payment and poor customer service</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1669,16 +1667,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>/users/6657780641e2bd610d7a03c4</t>
+          <t>/users/5db1f7d2a36427601bc23fc1</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Mr. Basheer Niravelil</t>
+          <t>Matthew Gaughran</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1688,18 +1686,23 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>I want to cancel the card</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
+          <t xml:space="preserve">Disgraceful </t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really unhappy. Loan ended and they still took a full payment! Had to contact them myself. Waited ages to speak to someone who struggled to understand me, there was a clear language barrier. The refund for the overpayment isn't instant and I have to wait for it. The advisor wasn't understanding or compassionate regarding the clear issue. Raised a complaint to be advised they have over 4 weeks to respond. Disgusting Update:A complaint was only raised today. Even though I asked the agent on the day to raise a complaint. Joke of a company.
+</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Basheer - I've asked a member of our Customer Support team to get in touch with you so that we can assist.Kind regards Sam Customer Engagement team.</t>
+Hi Matthew, thanks for the review.We're sorry to hear of the issues you've faced. We can see that a complaint has been raised and our Complaints team will be in touch in due course regarding your concerns.We can see that the payment was refunded the same day for you.LM</t>
         </is>
       </c>
       <c r="L22" s="2" t="n">
-        <v>45427</v>
+        <v>45446</v>
       </c>
     </row>
     <row r="23">
@@ -1713,25 +1716,25 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>terrible customer service</t>
+          <t>long wait times</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>/users/615b4c59d8211e0012c5630d</t>
+          <t>/users/6657780641e2bd610d7a03c4</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Mr. Basheer Niravelil</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1741,23 +1744,18 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Applied for a loan 5 days ago was…</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Applied for a loan 5 days ago was accepted and told it would be 24 hours for it to reach my account but I'm still waiting terrible customer service on app all it is is a bot that keeps telling me it doesn't understand my question.
-</t>
-        </is>
-      </c>
+          <t>I want to cancel the card</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Hi WIlliam - thanks for letting us know by leaving a review. I've sent you a request for more info so that we can get in touch and try to assist. </t>
+          <t>Reply from  118 118 MONEY
+Hi Basheer - I've asked a member of our Customer Support team to get in touch with you so that we can assist.Kind regards Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L23" s="2" t="n">
-        <v>45437</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="24">
@@ -1771,12 +1769,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>third time failed application</t>
+          <t>terrible customer service</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1784,12 +1782,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>/users/5f2445cbb15216fabf7d1b13</t>
+          <t>/users/615b4c59d8211e0012c5630d</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Edyta Baberska</t>
+          <t>William</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1799,23 +1797,23 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Ridiculous!!!</t>
+          <t>Applied for a loan 5 days ago was…</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t xml:space="preserve">For the 3rd time i received information that I am 100% approved for my credit card and when I try to apply , suddenly I am not. 3rd hard search on my history from 118 118 and no credit card. This is ridiculous!!!
+          <t xml:space="preserve">Applied for a loan 5 days ago was accepted and told it would be 24 hours for it to reach my account but I'm still waiting terrible customer service on app all it is is a bot that keeps telling me it doesn't understand my question.
 </t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hello Edyta - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me locate your application. SamCustomer Engagement team.</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Hi WIlliam - thanks for letting us know by leaving a review. I've sent you a request for more info so that we can get in touch and try to assist. </t>
         </is>
       </c>
       <c r="L24" s="2" t="n">
-        <v>45441</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="25">
@@ -1829,25 +1827,23 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>customer service problems and miscommunication</t>
+          <t>credit application failed again</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>customer service</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>1</v>
-      </c>
+          <t>application process</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>/users/5c640e15dfce6580e21cb2a1</t>
+          <t>/users/5f2445cbb15216fabf7d1b13</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>cameron clarke</t>
+          <t>Edyta Baberska</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1857,23 +1853,23 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shocking company don’t use </t>
+          <t>Ridiculous!!!</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t xml:space="preserve">I can’t actually believe how much of a scam this company is - all the customer service advisors appear to work from home and have no clue what they are doing. With so many issues in the past I thought I’d finally pay off my credit card and be done with them. I requested a settlement figure and the account to be closed - I went through the customer service team and was given a settlement figure of around £1600 which I paid and requested the account to be closed. I was advised this was all done. I have since been told that my account has not in fact been closed and they have since tried to bill me an extra 50 pound plus late payment fees. When speaking to the customer service team again I was told this is my fault and “I should have known that there would be another payment”. How would I have known this when I am told the account is closed? They refuse to take any responsibility for this and when I request a call back from a superior no one ever rings. I receive multiple automated calls a day hounding me about this but no calls from the customer service team. I can’t believe they are trying to scam me out of money and am honestly confused where all these positive reviews have come from as I have not had one positive experience from this company. 
+          <t xml:space="preserve">For the 3rd time i received information that I am 100% approved for my credit card and when I try to apply , suddenly I am not. 3rd hard search on my history from 118 118 and no credit card. This is ridiculous!!!
 </t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Cameron - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me identify your account. SamCustomer Engagement team.</t>
+Hello Edyta - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me locate your application. SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L25" s="2" t="n">
-        <v>45352</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="26">
@@ -1887,7 +1883,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>default notice after IVA settlement</t>
+          <t>scammed by customer service</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1895,15 +1891,17 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>/users/599c55470000ff000abeed0d</t>
+          <t>/users/5c640e15dfce6580e21cb2a1</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Mr Colin Moran</t>
+          <t>cameron clarke</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1913,18 +1911,23 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>I placed my credit card into an IVA</t>
+          <t xml:space="preserve">Shocking company don’t use </t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t xml:space="preserve">I placed my credit card into an IVA, so for 4 years 118 money didn't contact me.  My IVA was settled early in September 2023.  In March 118 money sent me a default notice for the reminder of the balance.  I have even sent the completion of the IVA with 118 money the first creditor.  The IVA is settled in court but 118 money are defaulting an account settled by court. The operator's on the phone couldn't understand the concept of the IVA.  They are now effecting my credit by adding miss payments , which they haven't added for 4 years. Don't trust this company
-</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
+          <t xml:space="preserve">I can’t actually believe how much of a scam this company is - all the customer service advisors appear to work from home and have no clue what they are doing. With so many issues in the past I thought I’d finally pay off my credit card and be done with them. I requested a settlement figure and the account to be closed - I went through the customer service team and was given a settlement figure of around £1600 which I paid and requested the account to be closed. I was advised this was all done. I have since been told that my account has not in fact been closed and they have since tried to bill me an extra 50 pound plus late payment fees. When speaking to the customer service team again I was told this is my fault and “I should have known that there would be another payment”. How would I have known this when I am told the account is closed? They refuse to take any responsibility for this and when I request a call back from a superior no one ever rings. I receive multiple automated calls a day hounding me about this but no calls from the customer service team. I can’t believe they are trying to scam me out of money and am honestly confused where all these positive reviews have come from as I have not had one positive experience from this company. 
+</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Reply from  118 118 MONEY
+Hello Cameron - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me identify your account. SamCustomer Engagement team.</t>
+        </is>
+      </c>
       <c r="L26" s="2" t="n">
-        <v>45439</v>
+        <v>45352</v>
       </c>
     </row>
     <row r="27">
@@ -1938,7 +1941,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>poor customer service</t>
+          <t>IVA settlement not recognized, default notice sent</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1946,17 +1949,15 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>1</v>
-      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>/users/66543821de93534aa0ffc632</t>
+          <t>/users/599c55470000ff000abeed0d</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Rebecca</t>
+          <t>Mr Colin Moran</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1966,23 +1967,18 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Credit card</t>
+          <t>I placed my credit card into an IVA</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Has a credit card a couple of years ago with this company and due to financial reasons got into arrears, 118 118 offered me to pay a reduced settlement sum which I did. Have all the emails to prove the the amount was paid and the account closed and that I will not be asked to pay the remaining amount! Last year I received legal letters from a debt collecting agency about paying off this debt, called 118 118 to find out what is going on they clarified that it has been paid, this year the same happends, being harrased with lots of phone calls daily, again rang 118 118 to find out what is going on still not heard anything back! This is appaling service.
-</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Reply from  118 118 MONEY
-Hello Rebecca - thank you for leaving a review and I am keen to investigate your comments. I have sent you a request for some information to enable that. Kind regards, Sam Customer Engagement team.</t>
-        </is>
-      </c>
+          <t xml:space="preserve">I placed my credit card into an IVA, so for 4 years 118 money didn't contact me.  My IVA was settled early in September 2023.  In March 118 money sent me a default notice for the reminder of the balance.  I have even sent the completion of the IVA with 118 money the first creditor.  The IVA is settled in court but 118 money are defaulting an account settled by court. The operator's on the phone couldn't understand the concept of the IVA.  They are now effecting my credit by adding miss payments , which they haven't added for 4 years. Don't trust this company
+</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" s="2" t="n">
-        <v>45436</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="28">
@@ -1996,7 +1992,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>harassment after paying early</t>
+          <t>poor customer service</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2009,12 +2005,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>/users/557dd0500000ff0001c5edef</t>
+          <t>/users/66543821de93534aa0ffc632</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Scotty</t>
+          <t>Rebecca</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2024,23 +2020,23 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Disgraceful Harrasment</t>
+          <t>Credit card</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Disgrace of a business.Entered an extremely short term payment arrangement with them due to delayed start date in a new job.I actually paid the arrangement EARLY but apparently this isn’t acceptable and as such, the harassment started.It is important you know this is not terminology, they have bombarded me with several hundred automated calls, texts and emails, some in earlyy hours of morning and sometimes 3 or 4 in an hour of work from different numbers. For paying EARLYI have compiled all off the data and information and am sending it as a pack the FSA and to anyone else I can think of that regulates financial services and telephone and digital communication, I must add I had never had a missed or late payment, and I contacted them well before any payments were due to inform them if the situation (I did this with 2 other companies I have financial accounts with, both of whom have been wonderful and I-have only had a single email from each, confirming-end date of agreement)This is the kindf harassment which could force someone with long term financial issues over the edge. I’m just happy that my issues was short term and that I do not have any kind of mental health issues.118 did try to get this review removed, unsurprisingly to me.Horrific company to deal with.
+          <t xml:space="preserve">Has a credit card a couple of years ago with this company and due to financial reasons got into arrears, 118 118 offered me to pay a reduced settlement sum which I did. Have all the emails to prove the the amount was paid and the account closed and that I will not be asked to pay the remaining amount! Last year I received legal letters from a debt collecting agency about paying off this debt, called 118 118 to find out what is going on they clarified that it has been paid, this year the same happends, being harrased with lots of phone calls daily, again rang 118 118 to find out what is going on still not heard anything back! This is appaling service.
 </t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Scotty - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me identify your account. We certainly take your comments in this review seriously.Sam Customer Engagement team.</t>
+Hello Rebecca - thank you for leaving a review and I am keen to investigate your comments. I have sent you a request for some information to enable that. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L28" s="2" t="n">
-        <v>45437</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="29">
@@ -2054,12 +2050,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>can't set up direct debit</t>
+          <t>harassment through automated calls/texts/emails</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -2067,12 +2063,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>/users/5d8bce472bfdf5daeb2b2bc0</t>
+          <t>/users/557dd0500000ff0001c5edef</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>wendy hart</t>
+          <t>Scotty</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2082,23 +2078,23 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>The app is rubbish I can't set up…</t>
+          <t>Disgraceful Harrasment</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t xml:space="preserve">The app is rubbish I can't set up direct debit I will not be using this credit card 
+          <t xml:space="preserve">Disgrace of a business.Entered an extremely short term payment arrangement with them due to delayed start date in a new job.I actually paid the arrangement EARLY but apparently this isn’t acceptable and as such, the harassment started.It is important you know this is not terminology, they have bombarded me with several hundred automated calls, texts and emails, some in earlyy hours of morning and sometimes 3 or 4 in an hour of work from different numbers. For paying EARLYI have compiled all off the data and information and am sending it as a pack the FSA and to anyone else I can think of that regulates financial services and telephone and digital communication, I must add I had never had a missed or late payment, and I contacted them well before any payments were due to inform them if the situation (I did this with 2 other companies I have financial accounts with, both of whom have been wonderful and I-have only had a single email from each, confirming-end date of agreement)This is the kindf harassment which could force someone with long term financial issues over the edge. I’m just happy that my issues was short term and that I do not have any kind of mental health issues.118 did try to get this review removed, unsurprisingly to me.Horrific company to deal with.
 </t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Thank you for leaving a review - I'm sorry to hear of your frustrations. I have asked a member of our Customer Support team to get in touch with you, so that we can try to assist. Kind regards, Sam Customer Engagement team.</t>
+Hello Scotty - thank you for leaving a review. I would like to investigate your comments and come back to you. I've sent a request for more information, to help me identify your account. We certainly take your comments in this review seriously.Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L29" s="2" t="n">
-        <v>45424</v>
+        <v>45437</v>
       </c>
     </row>
     <row r="30">
@@ -2112,12 +2108,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>declined without reason</t>
+          <t>can't set up direct debit</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>credit search problems</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -2125,12 +2121,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>/users/5d0056fcd2e77751643b8c58</t>
+          <t>/users/5d8bce472bfdf5daeb2b2bc0</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>David Adams</t>
+          <t>wendy hart</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2140,23 +2136,23 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guaranteed loan.....Declined!! </t>
+          <t>The app is rubbish I can't set up…</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t xml:space="preserve">I've had a credit card with 118 for over 5 years. I've had 2 limit increases over that period to 1,200.Never missed a payment or late etc.Logged in to the App yesterday, saying I was pre-approved for a loan of £2,500 over 3 years.As I say only pre-approved so I know I could still be declined.Went through the first bit....congratulations, your are GUARANTEED for a loan of £2,500 with the information you've provided.Next stage, verified my debit card and bank account.Then it provided me with the agreement, T&amp;Cs etc. First repayment date 1st July.Brilliant, I thought....just sign and submit.....DECLINED!!?? How?? Called customer service and although very polite and helpful, no real reason  was provided! **Update** just checked my credit file and not only a soft search completed by them, also a hard search!??Usually when companies do hard searches it means they will lend to you...obviously not in 118's case!! 
+          <t xml:space="preserve">The app is rubbish I can't set up direct debit I will not be using this credit card 
 </t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Thank you for leaving a review. I would like to investigate this further for you and have sent a request for more information.Kind regards,SamCustomer Engagement team.</t>
+Thank you for leaving a review - I'm sorry to hear of your frustrations. I have asked a member of our Customer Support team to get in touch with you, so that we can try to assist. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L30" s="2" t="n">
-        <v>45433</v>
+        <v>45424</v>
       </c>
     </row>
     <row r="31">
@@ -2170,7 +2166,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>credit file affected by company's actions</t>
+          <t>declined without reason</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2183,12 +2179,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>/users/563a4ff30000ff0001e8235b</t>
+          <t>/users/5d0056fcd2e77751643b8c58</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Edward Mawby</t>
+          <t>David Adams</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2198,23 +2194,23 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Terrible company</t>
+          <t xml:space="preserve">Guaranteed loan.....Declined!! </t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Terrible company. I had used this company in the past and tried to get a loan. Did a simple check and said I was guaranteed, signed the documents did all the other checks and then came back declined. The worst bit was they had the cheek of putting a hard check on my credit file which will now affect any other applications I try to do. Avoid at all costs.
+          <t xml:space="preserve">I've had a credit card with 118 for over 5 years. I've had 2 limit increases over that period to 1,200.Never missed a payment or late etc.Logged in to the App yesterday, saying I was pre-approved for a loan of £2,500 over 3 years.As I say only pre-approved so I know I could still be declined.Went through the first bit....congratulations, your are GUARANTEED for a loan of £2,500 with the information you've provided.Next stage, verified my debit card and bank account.Then it provided me with the agreement, T&amp;Cs etc. First repayment date 1st July.Brilliant, I thought....just sign and submit.....DECLINED!!?? How?? Called customer service and although very polite and helpful, no real reason  was provided! **Update** just checked my credit file and not only a soft search completed by them, also a hard search!??Usually when companies do hard searches it means they will lend to you...obviously not in 118's case!! 
 </t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Thank you for leaving a review and for responding to our request for further info. I am inviestigating your comments and will come back to you with an update.Kind regards, Sam Customer Engagement team.</t>
+Thank you for leaving a review. I would like to investigate this further for you and have sent a request for more information.Kind regards,SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L31" s="2" t="n">
-        <v>45430</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="32">
@@ -2228,12 +2224,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>unfair business practices</t>
+          <t>declined loan after signing documents</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>credit search problems</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -2241,12 +2237,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>/users/608860bc290f8a0019269ac0</t>
+          <t>/users/563a4ff30000ff0001e8235b</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Scaramanga </t>
+          <t>Edward Mawby</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2256,23 +2252,23 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Total scumbags preying on vulnerable…</t>
+          <t>Terrible company</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Total scumbags preying on vulnerable people. Do everything they can to get you into a cycle of high interest debt. Don't be fooled by the light hearted marketing, this company are bullying crooks who will hopefully go the way of Amigo and others soon. You have been warned....Edit: in response to the below, I already complained and 118118money took an age to respond and then sent me a derogatory and condescending final response. Don't waste your time.
+          <t xml:space="preserve">Terrible company. I had used this company in the past and tried to get a loan. Did a simple check and said I was guaranteed, signed the documents did all the other checks and then came back declined. The worst bit was they had the cheek of putting a hard check on my credit file which will now affect any other applications I try to do. Avoid at all costs.
 </t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - I am sorry to see these comments. I have sent you a request for more information, so that I can investigate this for you. Otherwise, you can contact complaints@118118money.com and we'll look into your concerns.Kind regards, Sam Customer Engagement team.</t>
+Thank you for leaving a review and for responding to our request for further info. I am inviestigating your comments and will come back to you with an update.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L32" s="2" t="n">
-        <v>45427</v>
+        <v>45430</v>
       </c>
     </row>
     <row r="33">
@@ -2286,12 +2282,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>pre-approval despite being told cannot reapply</t>
+          <t>company is dishonest and unresponsive</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -2299,12 +2295,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>/users/663ce7a6b55dd36b50ae4dd0</t>
+          <t>/users/608860bc290f8a0019269ac0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Stuart</t>
+          <t xml:space="preserve">Scaramanga </t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2314,23 +2310,23 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Repeatedly telling me I am pre-approved and then rejecting me!</t>
+          <t>Total scumbags preying on vulnerable…</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t xml:space="preserve">I had a loan with 118 that I paid off early. I reapplied in January and was rejected for unknown reasons but then the next day I received an email saying I was preapproved. I tried to apply but page wouldn't load and customer services told me that I couldn't reapply for 180 days.Roll on to now and I get another 'pre-approved' email for a larger amount - still unable to access the offer.Is it me or should they not send you these if they have told you you can't reapply for a certain length of time?!I wouldn't mind but paid 1st loan off early and was always on time with payments.Customer service don't care!
+          <t xml:space="preserve">Total scumbags preying on vulnerable people. Do everything they can to get you into a cycle of high interest debt. Don't be fooled by the light hearted marketing, this company are bullying crooks who will hopefully go the way of Amigo and others soon. You have been warned....Edit: in response to the below, I already complained and 118118money took an age to respond and then sent me a derogatory and condescending final response. Don't waste your time.
 </t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Stuart - I'm sorry to hear you're frsutrated and thank you for leaving for a review. I have sent you a request for more information, so that we can look into this for you. Kind regardsSam Customer Engagement team.</t>
+Hello - I am sorry to see these comments. I have sent you a request for more information, so that I can investigate this for you. Otherwise, you can contact complaints@118118money.com and we'll look into your concerns.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L33" s="2" t="n">
-        <v>45421</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="34">
@@ -2344,12 +2340,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>delayed delivery</t>
+          <t>preapproval despite being told to reapply later</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>speed</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -2357,12 +2353,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>/users/663c73d7cb98c55959de5a60</t>
+          <t>/users/663ce7a6b55dd36b50ae4dd0</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Riggz</t>
+          <t>Stuart</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2372,23 +2368,23 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Still not even received my card or pin…</t>
+          <t>Repeatedly telling me I am pre-approved and then rejecting me!</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Still not even received my card or pin number!
+          <t xml:space="preserve">I had a loan with 118 that I paid off early. I reapplied in January and was rejected for unknown reasons but then the next day I received an email saying I was preapproved. I tried to apply but page wouldn't load and customer services told me that I couldn't reapply for 180 days.Roll on to now and I get another 'pre-approved' email for a larger amount - still unable to access the offer.Is it me or should they not send you these if they have told you you can't reapply for a certain length of time?!I wouldn't mind but paid 1st loan off early and was always on time with payments.Customer service don't care!
 </t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi - I have asked a member of our Customer Support team to get in contact with you to discuss this.Kind regardsSamCustomer Engagement team</t>
+Hi Stuart - I'm sorry to hear you're frsutrated and thank you for leaving for a review. I have sent you a request for more information, so that we can look into this for you. Kind regardsSam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L34" s="2" t="n">
-        <v>45414</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="35">
@@ -2402,25 +2398,25 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>unhelpful customer service</t>
+          <t>did not receive card or pin</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>/users/6366d5d4a273830012228617</t>
+          <t>/users/663c73d7cb98c55959de5a60</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>John sheehan</t>
+          <t>Riggz</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2430,18 +2426,23 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>No credit card 10days</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr"/>
+          <t>Still not even received my card or pin…</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still not even received my card or pin number!
+</t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Hi John - I have asked a member of our Customer Support team to get in contact with you to discuss this. Kind regards Sam Customer Engagement team </t>
+          <t>Reply from  118 118 MONEY
+Hi - I have asked a member of our Customer Support team to get in contact with you to discuss this.Kind regardsSamCustomer Engagement team</t>
         </is>
       </c>
       <c r="L35" s="2" t="n">
-        <v>45411</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="36">
@@ -2455,25 +2456,25 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>loan payment taken twice, no rush to refund</t>
+          <t>credit search issues</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>credit search problems</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>/users/5c0d2cf63f0baa15172918c7</t>
+          <t>/users/6366d5d4a273830012228617</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>tronayne451</t>
+          <t>John sheehan</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2483,23 +2484,18 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Taken payment twice</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Unfortunately after having numerous problems with this company which to be fair I was apologised to and compensated at least in respect of my credit card account was enough for me to remove my previous negative reviews about them.However my loan payment has now been taken twice and although acknowledging that this has happened they appear in no rush to refund the money to me.  Whilst understanding that mistakes do happen the money should have been back in my account the same day.Another very poor performance that falls well  below FCA principle 12 Consumer Duty obtaining a good outcome for retail customers.Hopefully at some stage when it suits them they will refund the money that they have wrongly taken from my account.
-</t>
-        </is>
-      </c>
+          <t>No credit card 10days</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hi there - thank you for leaving a review - I'd like to investigate this as quickly as possible for  you. I've sent a request for info, so that I can locate your account. Kind regards Sam Customer Engagement team,</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Hi John - I have asked a member of our Customer Support team to get in contact with you to discuss this. Kind regards Sam Customer Engagement team </t>
         </is>
       </c>
       <c r="L36" s="2" t="n">
-        <v>45414</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="37">
@@ -2513,12 +2509,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>money management is shameless</t>
+          <t>refund issues with loan payment</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>issues on holiday</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -2526,12 +2522,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>/users/54f59c2d0000ff0001aeb8da</t>
+          <t>/users/5c0d2cf63f0baa15172918c7</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Ian Purdy</t>
+          <t>tronayne451</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2541,23 +2537,23 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1% shylocks</t>
+          <t>Taken payment twice</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t xml:space="preserve">99%.  Money whores. Shameless. 
+          <t xml:space="preserve">Unfortunately after having numerous problems with this company which to be fair I was apologised to and compensated at least in respect of my credit card account was enough for me to remove my previous negative reviews about them.However my loan payment has now been taken twice and although acknowledging that this has happened they appear in no rush to refund the money to me.  Whilst understanding that mistakes do happen the money should have been back in my account the same day.Another very poor performance that falls well  below FCA principle 12 Consumer Duty obtaining a good outcome for retail customers.Hopefully at some stage when it suits them they will refund the money that they have wrongly taken from my account.
 </t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Ian - If there is something specific that you're unhappy with, we would be keen to understand what that is. Please contact us  via chat function in the app or by calling us on 02920 548 118.RegardsCustomer Engagement team</t>
+Hi there - thank you for leaving a review - I'd like to investigate this as quickly as possible for  you. I've sent a request for info, so that I can locate your account. Kind regards Sam Customer Engagement team,</t>
         </is>
       </c>
       <c r="L37" s="2" t="n">
-        <v>45411</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="38">
@@ -2571,7 +2567,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>chat resolution failed</t>
+          <t>money whores shameless</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2579,15 +2575,17 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>/users/5f06ec9e866c46f5793c4269</t>
+          <t>/users/54f59c2d0000ff0001aeb8da</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Shane</t>
+          <t>Ian Purdy</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2597,23 +2595,23 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>I recently contacted an agent via the…</t>
+          <t>1% shylocks</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t xml:space="preserve">I recently contacted an agent via the chat, nothing was resolved and he left the chat lea in me rather frustrated 
+          <t xml:space="preserve">99%.  Money whores. Shameless. 
 </t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Hi Shane - I'm sorry to hear you're not happy. I have asked a member of the Customer Support team to contact you to try and resolve any issues you have.Kind regards Sam Customer Engagement team. </t>
+          <t>Reply from  118 118 MONEY
+Hi Ian - If there is something specific that you're unhappy with, we would be keen to understand what that is. Please contact us  via chat function in the app or by calling us on 02920 548 118.RegardsCustomer Engagement team</t>
         </is>
       </c>
       <c r="L38" s="2" t="n">
-        <v>45416</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="39">
@@ -2627,12 +2625,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>app doesn't work abroad</t>
+          <t>agent unhelpful</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>issues on holiday</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -2640,12 +2638,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>/users/62aca5900a6f7400134ed115</t>
+          <t>/users/5f06ec9e866c46f5793c4269</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Yvonne</t>
+          <t>Shane</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2655,23 +2653,23 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>App and website does not work outside of UK</t>
+          <t>I recently contacted an agent via the…</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Love my 118 in UK as the App is good. Gone on holiday and wasted so much time trying to open the app eventually decided to phone and was told that the app and website does not work outside the UK - absolutely useless 🤬 travelling is when you need the app the most. 
+          <t xml:space="preserve">I recently contacted an agent via the chat, nothing was resolved and he left the chat lea in me rather frustrated 
 </t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hi Yvonne - I'm sorry to hear you found this frustrating. I will look into this and raise your feedback. Thank you for leaving us a review.Kind regards Sam Customer Engagement team.</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Hi Shane - I'm sorry to hear you're not happy. I have asked a member of the Customer Support team to contact you to try and resolve any issues you have.Kind regards Sam Customer Engagement team. </t>
         </is>
       </c>
       <c r="L39" s="2" t="n">
-        <v>45418</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="40">
@@ -2685,12 +2683,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>harassment by calls and emails</t>
+          <t>app doesn't work abroad</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>issues on holiday</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -2698,12 +2696,12 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>/users/5c76f6461652bb5feea4055c</t>
+          <t>/users/62aca5900a6f7400134ed115</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Feena</t>
+          <t>Yvonne</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2713,23 +2711,23 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>After weeks of trying to arrange a…</t>
+          <t>App and website does not work outside of UK</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t xml:space="preserve">After weeks of trying to arrange a payment plan, I finally managed to get it sorted, but only after leaving a negative review on here and being contacted by a 118 staff member who saw my feedback.I thought everything was sorted, as I managed to get a monthly payment plan agreed.However, after only two months of the plan running, I am now being harrassed by 118 calls and emails, pressuring me to settle my arrears.Legally, this should not happen when a payment plan is in place.118 customer service are not answering my emails, so maybe a 118 staff member will see this negative review again and help me get this sorted?????
+          <t xml:space="preserve">Love my 118 in UK as the App is good. Gone on holiday and wasted so much time trying to open the app eventually decided to phone and was told that the app and website does not work outside the UK - absolutely useless 🤬 travelling is when you need the app the most. 
 </t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Hello Feena - I am sorry to hear that you are having trouble contacting us. I have sent you a request for more information so that I can look into why this is and also arrange for a member of the Customer Support team to contact you. </t>
+          <t>Reply from  118 118 MONEY
+Hi Yvonne - I'm sorry to hear you found this frustrating. I will look into this and raise your feedback. Thank you for leaving us a review.Kind regards Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L40" s="2" t="n">
-        <v>45416</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="41">
@@ -2738,28 +2736,30 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>medical evidence required</t>
+          <t>harassment after payment plan set up</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>application process</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>customer service</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>/users/609a9945910779001a954693</t>
+          <t>/users/5c76f6461652bb5feea4055c</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Leon</t>
+          <t>Feena</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2769,23 +2769,23 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Irresponsibly</t>
+          <t>After weeks of trying to arrange a…</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t xml:space="preserve">IrresponsiblyLent me the money please see my Medical evidence
+          <t xml:space="preserve">After weeks of trying to arrange a payment plan, I finally managed to get it sorted, but only after leaving a negative review on here and being contacted by a 118 staff member who saw my feedback.I thought everything was sorted, as I managed to get a monthly payment plan agreed.However, after only two months of the plan running, I am now being harrassed by 118 calls and emails, pressuring me to settle my arrears.Legally, this should not happen when a payment plan is in place.118 customer service are not answering my emails, so maybe a 118 staff member will see this negative review again and help me get this sorted?????
 </t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hi Leon - please contact us if you would like to discuss withdrawing from the agreement. Our Customer Support team is available to help you with this. Please chat in the app or call us on 02920 548 118.Sam Customer Engagement team.</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Hello Feena - I am sorry to hear that you are having trouble contacting us. I have sent you a request for more information so that I can look into why this is and also arrange for a member of the Customer Support team to contact you. </t>
         </is>
       </c>
       <c r="L41" s="2" t="n">
-        <v>45413</v>
+        <v>45416</v>
       </c>
     </row>
     <row r="42">
@@ -2799,12 +2799,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>application process smooth</t>
+          <t>getting loan quickly</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -2812,12 +2812,12 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>/users/632df76c44d1f30012c6891c</t>
+          <t>/users/609a9945910779001a954693</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Samuel Windrim</t>
+          <t>Leon</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2827,23 +2827,23 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Sorry i meant to hit 5 stars not 1…</t>
+          <t>Irresponsibly</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sorry i meant to hit 5 stars not 1 application process was fine no hassle and so far everything good so would recommend 118 in future to friends and family
+          <t xml:space="preserve">IrresponsiblyLent me the money please see my Medical evidence
 </t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Thanks Samuel - we appreciate the feedback. Please feel free to amend your rating accordingly :) Thanks for being a 118 118 Money customer.Sam Customer Engagement team. </t>
+          <t>Reply from  118 118 MONEY
+Hi Leon - please contact us if you would like to discuss withdrawing from the agreement. Our Customer Support team is available to help you with this. Please chat in the app or call us on 02920 548 118.Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L42" s="2" t="n">
-        <v>45415</v>
+        <v>45413</v>
       </c>
     </row>
     <row r="43">
@@ -2852,30 +2852,30 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>identity theft</t>
+          <t>application process easy</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>credit search problems</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>/users/62e91fd7b6b8ff00124dfe38</t>
+          <t>/users/632df76c44d1f30012c6891c</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Leonard Strike</t>
+          <t>Samuel Windrim</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2885,23 +2885,23 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Someone took a loan out in my name I'm…</t>
+          <t>Sorry i meant to hit 5 stars not 1…</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Someone took a loan out in my name I'm not happy someone used my identity. 
+          <t xml:space="preserve">Sorry i meant to hit 5 stars not 1 application process was fine no hassle and so far everything good so would recommend 118 in future to friends and family
 </t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hello Leonard - thank you for letting us know. I have passed your details to our Financial Crime team so we can help you resolve this.Sam Customer Engagement team</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Thanks Samuel - we appreciate the feedback. Please feel free to amend your rating accordingly :) Thanks for being a 118 118 Money customer.Sam Customer Engagement team. </t>
         </is>
       </c>
       <c r="L43" s="2" t="n">
-        <v>45406</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="44">
@@ -2915,12 +2915,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>no payment received</t>
+          <t>identity theft issue</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2928,12 +2928,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>/users/66327ee5ed4fa10012fcc12d</t>
+          <t>/users/62e91fd7b6b8ff00124dfe38</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Mr. Darren Longstaff</t>
+          <t>Leonard Strike</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2943,18 +2943,23 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>No payment received</t>
+          <t>Someone took a loan out in my name I'm…</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t xml:space="preserve">No payment received 
-</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
+          <t xml:space="preserve">Someone took a loan out in my name I'm not happy someone used my identity. 
+</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Reply from  118 118 MONEY
+Hello Leonard - thank you for letting us know. I have passed your details to our Financial Crime team so we can help you resolve this.Sam Customer Engagement team</t>
+        </is>
+      </c>
       <c r="L44" s="2" t="n">
-        <v>45413</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="45">
@@ -2968,12 +2973,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>pre-approval doesn't mean guaranteed loan approval</t>
+          <t>no payment received</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>credit search problems</t>
+          <t>speed</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2981,12 +2986,12 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>/users/63a9c51b7fe302001306672b</t>
+          <t>/users/66327ee5ed4fa10012fcc12d</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Terence B.</t>
+          <t>Mr. Darren Longstaff</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2996,23 +3001,18 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>No idea what’s going on</t>
+          <t>No payment received</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t xml:space="preserve">I am constantly told I’m pre-approved and “triple lock guaranteed” for loans, so I run the search and get hard searches for no reason because ultimately, the loans are always declined.I have no idea why I’m even pre-approved if this always happens. It’s a bit crazy.
-</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Reply from  118 118 MONEY
-Hi Terence - thank you for leaving a review. I have sent you a request for more information, so that we can look into this for you.Kind regards, Sam Customer Engagement team.</t>
-        </is>
-      </c>
+          <t xml:space="preserve">No payment received 
+</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
       <c r="L45" s="2" t="n">
-        <v>45403</v>
+        <v>45413</v>
       </c>
     </row>
     <row r="46">
@@ -3026,12 +3026,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>poor customer service</t>
+          <t>constant false promises of approval</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>application process</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -3039,12 +3039,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>/users/59563d8d0000ff000aa9f1cf</t>
+          <t>/users/63a9c51b7fe302001306672b</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Luke Bruce</t>
+          <t>Terence B.</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3054,23 +3054,23 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Horrendous service and horrendous app. Avoid avoid avoid</t>
+          <t>No idea what’s going on</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horrendous service and horrendous app. Stay well clear.Yet again I am having issues. My apps balance is about £200 out of sync but I have only made 3 transactions in the last week or so and they only total to about £50.I have been on phone for 30 mins because the advisor cannot answer any simple questions. They hung up or the call dropped. They didn't attempt to call back unsurprisingly.I will make an official complaint but like the last one they will probably take 7 weeks to reply and not allow any opportunity for dialogue and go straight to final response.I really regret giving these guys a chance. Out of all competitors I've used these guys are by far the worse in all areas. They do nothing well. I recommend you choose any card but these. Their rates aren't great so there is no upside.Trust pilot should allow 0 stars as there is no way 118 deserve a 1 star
+          <t xml:space="preserve">I am constantly told I’m pre-approved and “triple lock guaranteed” for loans, so I run the search and get hard searches for no reason because ultimately, the loans are always declined.I have no idea why I’m even pre-approved if this always happens. It’s a bit crazy.
 </t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Luke - I'm sorry to hear that you're not happy with our service. You've noted that you will be making a complaint. If you haven't already, you can do so, by sending an email to: complaints@118118money.com. Sam Customer Engagement team.</t>
+Hi Terence - thank you for leaving a review. I have sent you a request for more information, so that we can look into this for you.Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L46" s="2" t="n">
-        <v>45411</v>
+        <v>45403</v>
       </c>
     </row>
     <row r="47">
@@ -3084,12 +3084,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>issues with card payment abroad</t>
+          <t>poor customer service and app issues</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -3097,12 +3097,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>/users/636702ed98da2300124ce118</t>
+          <t>/users/59563d8d0000ff000aa9f1cf</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Mr Allen-Khimani</t>
+          <t>Luke Bruce</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3112,23 +3112,23 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>I was abroad and had an issue with a…</t>
+          <t>Horrendous service and horrendous app. Avoid avoid avoid</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t xml:space="preserve">I was abroad and had an issue with a card payment (I had plenty of credit on my card). Tried to instant message you to which you said you could not help and closed the chat down. The oversea number given did not connect - I tired about 5 times. Used a different provider. 
+          <t xml:space="preserve">Horrendous service and horrendous app. Stay well clear.Yet again I am having issues. My apps balance is about £200 out of sync but I have only made 3 transactions in the last week or so and they only total to about £50.I have been on phone for 30 mins because the advisor cannot answer any simple questions. They hung up or the call dropped. They didn't attempt to call back unsurprisingly.I will make an official complaint but like the last one they will probably take 7 weeks to reply and not allow any opportunity for dialogue and go straight to final response.I really regret giving these guys a chance. Out of all competitors I've used these guys are by far the worse in all areas. They do nothing well. I recommend you choose any card but these. Their rates aren't great so there is no upside.Trust pilot should allow 0 stars as there is no way 118 deserve a 1 star
 </t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi - thank you for leaving a review. I am sorry to hear you had difficulty chatting to us. I will look into this and a member of the team will come back to you.</t>
+Hi Luke - I'm sorry to hear that you're not happy with our service. You've noted that you will be making a complaint. If you haven't already, you can do so, by sending an email to: complaints@118118money.com. Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L47" s="2" t="n">
-        <v>45394</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="48">
@@ -3137,30 +3137,30 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>good customer service</t>
+          <t>issue with card payment while abroad</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>account access</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>/users/5d975f09dfffa8147d6671cf</t>
+          <t>/users/636702ed98da2300124ce118</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Mr Virgilio Pereira.</t>
+          <t>Mr Allen-Khimani</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3170,23 +3170,23 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Good Customer Service</t>
+          <t>I was abroad and had an issue with a…</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Good Customer Service 
+          <t xml:space="preserve">I was abroad and had an issue with a card payment (I had plenty of credit on my card). Tried to instant message you to which you said you could not help and closed the chat down. The oversea number given did not connect - I tired about 5 times. Used a different provider. 
 </t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Thanks for leaving us a review - we're glad you think the customer service we provide is good. Although, it looks like you might have selected the wrong rating!</t>
+Hi - thank you for leaving a review. I am sorry to hear you had difficulty chatting to us. I will look into this and a member of the team will come back to you.</t>
         </is>
       </c>
       <c r="L48" s="2" t="n">
-        <v>45409</v>
+        <v>45394</v>
       </c>
     </row>
     <row r="49">
@@ -3195,30 +3195,30 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>problems logging in</t>
+          <t>good customer service</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>account access</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>/users/5edcb71038d546276cf14cf9</t>
+          <t>/users/5d975f09dfffa8147d6671cf</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Lambros Chudley</t>
+          <t>Mr Virgilio Pereira.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3228,23 +3228,23 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>I have not yet received my card over a…</t>
+          <t>Good Customer Service</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">I have not yet received my card over a week later. When I try to log into my account using your app it asks for a password but will not let me use the numerical keypad. So far I would say the experience has been totally awful and I will be sharing this impression with my friends
+          <t xml:space="preserve">Good Customer Service 
 </t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Lambros - thanks for leaving us a review. I can see that you have now spoken to our Customer Support team and this has been resolved. Kind regards, SamCustomer Engagement team.</t>
+Thanks for leaving us a review - we're glad you think the customer service we provide is good. Although, it looks like you might have selected the wrong rating!</t>
         </is>
       </c>
       <c r="L49" s="2" t="n">
-        <v>45401</v>
+        <v>45409</v>
       </c>
     </row>
     <row r="50">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>funds didn't arrive in bank</t>
+          <t>account login issues</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -3271,12 +3271,12 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>/users/662bbfeb807e720012df0112</t>
+          <t>/users/5edcb71038d546276cf14cf9</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Cal</t>
+          <t>Lambros Chudley</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3286,23 +3286,23 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Never received the money </t>
+          <t>I have not yet received my card over a…</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Approved my loan, direct debit set up, balance of my loan in the app, agreement signed, and yet the loan never arrived in my bank accountNow been 3 weeks since I was approved and everything was signed and set up, and yet still, the funds have not arrived in my bank account
+          <t xml:space="preserve">I have not yet received my card over a week later. When I try to log into my account using your app it asks for a password but will not let me use the numerical keypad. So far I would say the experience has been totally awful and I will be sharing this impression with my friends
 </t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi - Thank you for leaving a review for us. I can see that you have raised this with our Complaints team and an investigation is underway. Kind regards, Sam Customer Engagement team.</t>
+Hi Lambros - thanks for leaving us a review. I can see that you have now spoken to our Customer Support team and this has been resolved. Kind regards, SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L50" s="2" t="n">
-        <v>45408</v>
+        <v>45401</v>
       </c>
     </row>
     <row r="51">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>credit card blocked with no response</t>
+          <t>loan didn't arrive after approval</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -3329,12 +3329,12 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>/users/649beb9ce5d57f0012a059d2</t>
+          <t>/users/662bbfeb807e720012df0112</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Stephen Harding</t>
+          <t>Cal</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3344,19 +3344,19 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>Credit card blocked no response</t>
+          <t xml:space="preserve">Never received the money </t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Credit card blocked no response 
+          <t xml:space="preserve">Approved my loan, direct debit set up, balance of my loan in the app, agreement signed, and yet the loan never arrived in my bank accountNow been 3 weeks since I was approved and everything was signed and set up, and yet still, the funds have not arrived in my bank account
 </t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Stephen - thanks for your review. I have sent you a request for more information, so that we can look into this for you.Sam Customer Engagement team.</t>
+Hi - Thank you for leaving a review for us. I can see that you have raised this with our Complaints team and an investigation is underway. Kind regards, Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L51" s="2" t="n">
@@ -3374,12 +3374,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Poor customer support and lack of interest</t>
+          <t>credit card blocked with no response</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>customer service</t>
+          <t>account access</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -3387,12 +3387,12 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>/users/606889baa97e40001b8bff43</t>
+          <t>/users/649beb9ce5d57f0012a059d2</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Steven Scorer</t>
+          <t>Stephen Harding</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3402,23 +3402,23 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Zero interest in customers </t>
+          <t>Credit card blocked no response</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Update! Take zero notice of the company replies to people's reviews as shown on my last review it states " A customer support member will contact you" as of yet no one has and the phone call today was a waste of time again when asked why the loan hasn't been transferred "I don't know" was the reply from the agent! I was then told "Just wait, it will get to you maybe next week" is that what you call customer support?? Your company is a joke and don't bother replying with your standard s**t "we are sorry" sorry for what your lack of interest in your customers? Or sorry for your s**t company? 2 to 24hrs your website states I'm sitting on 72hrs as of now!! Companies a joke end of story will tell anyone I can to avoid you's at all cost 
+          <t xml:space="preserve">Credit card blocked no response 
 </t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-We're sorry to hear you weren't happy with our service. I can see that the matter has now been closed.Customer Engagement team.</t>
+Hi Stephen - thanks for your review. I have sent you a request for more information, so that we can look into this for you.Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L52" s="2" t="n">
-        <v>45407</v>
+        <v>45408</v>
       </c>
     </row>
     <row r="53">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>poor customer service</t>
+          <t>poor customer support</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -3460,23 +3460,23 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Worst company I've taken a personal loan with </t>
+          <t xml:space="preserve">Zero interest in customers </t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Worst company I've taken a personal loan with customer service are extremely poor, when asked a question the response was I don't know.... the silence. Three days have passed since I took the personal loan and as of yet I haven't received the loan, as stated the service is a joke would avoid this company like a dose of the clap 
+          <t xml:space="preserve">Update! Take zero notice of the company replies to people's reviews as shown on my last review it states " A customer support member will contact you" as of yet no one has and the phone call today was a waste of time again when asked why the loan hasn't been transferred "I don't know" was the reply from the agent! I was then told "Just wait, it will get to you maybe next week" is that what you call customer support?? Your company is a joke and don't bother replying with your standard s**t "we are sorry" sorry for what your lack of interest in your customers? Or sorry for your s**t company? 2 to 24hrs your website states I'm sitting on 72hrs as of now!! Companies a joke end of story will tell anyone I can to avoid you's at all cost 
 </t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Steven. I'm sorry to hear that you're having difficulty. Thank you for leaving the review. I have asked a member of our Customer Support team to get in contact with you to get this resolved. Kind regards,Sam Customer Engagement team.</t>
+We're sorry to hear you weren't happy with our service. I can see that the matter has now been closed.Customer Engagement team.</t>
         </is>
       </c>
       <c r="L53" s="2" t="n">
-        <v>45405</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="54">
@@ -3485,30 +3485,30 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>easy application process</t>
+          <t>poor customer service</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>application process</t>
+          <t>customer service</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>/users/6628aaf4e7c8e4001225c8d3</t>
+          <t>/users/606889baa97e40001b8bff43</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Mr. John Taylor</t>
+          <t>Steven Scorer</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3518,18 +3518,23 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Haven’t received card or pin</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr"/>
+          <t xml:space="preserve">Worst company I've taken a personal loan with </t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Worst company I've taken a personal loan with customer service are extremely poor, when asked a question the response was I don't know.... the silence. Three days have passed since I took the personal loan and as of yet I haven't received the loan, as stated the service is a joke would avoid this company like a dose of the clap 
+</t>
+        </is>
+      </c>
       <c r="K54" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi John - thanks for your review. I can see that you're still in the ten days we advise it can take for your card to arrive. If you still haven't received your card after that ten days, please do let us know.Sam Customer Engagement team.</t>
+Hi Steven. I'm sorry to hear that you're having difficulty. Thank you for leaving the review. I have asked a member of our Customer Support team to get in contact with you to get this resolved. Kind regards,Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L54" s="2" t="n">
-        <v>45399</v>
+        <v>45405</v>
       </c>
     </row>
     <row r="55">
@@ -3543,7 +3548,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>no reason for blocking</t>
+          <t>delayed response</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3552,16 +3557,16 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>/users/649beb9ce5d57f0012a059d2</t>
+          <t>/users/6628aaf4e7c8e4001225c8d3</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Stephen Harding</t>
+          <t>Mr. John Taylor</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3571,23 +3576,18 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Blocked my card no reason no…</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Blocked my card no reason no communication sent me a new card but cart use it
-</t>
-        </is>
-      </c>
+          <t>Haven’t received card or pin</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Stephen - if we blocked your card, this will have been for a valid reason. I've sent you a request for more info, so that a member of our Customer Support team can reach out to try and assist.Kind regards Sam Customer Engagement team.</t>
+Hi John - thanks for your review. I can see that you're still in the ten days we advise it can take for your card to arrive. If you still haven't received your card after that ten days, please do let us know.Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L55" s="2" t="n">
-        <v>45402</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="56">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>inaccurate billing notifications</t>
+          <t>no communication or explanation</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3609,15 +3609,17 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>/users/566a9d390000ff0001f26b4a</t>
+          <t>/users/649beb9ce5d57f0012a059d2</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Stephen Harding</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3627,23 +3629,23 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Poor I.T set up and customer service</t>
+          <t>Blocked my card no reason no…</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t xml:space="preserve">I continually receive emails telling me to pay my bill when I have already.  I continually receive emails telling me I've missed my payment when I haven't.  FYI I pay by Direct Debit. 
+          <t xml:space="preserve">Blocked my card no reason no communication sent me a new card but cart use it
 </t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Chris - I have looked into this for you. I think there may be some confusion here, we are aware that your account is up to date. If you have any questions about a communication you have received, please contact our Customer Support team on 02920 548 118 or chat to us in the app.Thanks for being a 118 118 Money customer.SamCustomer Engagement team.</t>
+Hi Stephen - if we blocked your card, this will have been for a valid reason. I've sent you a request for more info, so that a member of our Customer Support team can reach out to try and assist.Kind regards Sam Customer Engagement team.</t>
         </is>
       </c>
       <c r="L56" s="2" t="n">
-        <v>45362</v>
+        <v>45402</v>
       </c>
     </row>
     <row r="57">
@@ -3657,7 +3659,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>constant unwanted calls</t>
+          <t>receiving incorrect payment reminders</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -3665,17 +3667,15 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E57" t="n">
-        <v>1</v>
-      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>/users/5e2a072261678140a2874591</t>
+          <t>/users/566a9d390000ff0001f26b4a</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>T Hu5541n</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3685,23 +3685,23 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>I've just had over 20 calls from 118…</t>
+          <t>Poor I.T set up and customer service</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t xml:space="preserve">I've just had over 20 calls from 118 118 money non stop over a couple of hours today Friday Afternoon. This is highly suspicious and they will NOT stop ringing me.
+          <t xml:space="preserve">I continually receive emails telling me to pay my bill when I have already.  I continually receive emails telling me I've missed my payment when I haven't.  FYI I pay by Direct Debit. 
 </t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello - I would like to look into this for you - thank you for your review. Please provide some more info to enable us to investigate your complaint.SamCustomer Engagement team.</t>
+Hi Chris - I have looked into this for you. I think there may be some confusion here, we are aware that your account is up to date. If you have any questions about a communication you have received, please contact our Customer Support team on 02920 548 118 or chat to us in the app.Thanks for being a 118 118 Money customer.SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L57" s="2" t="n">
-        <v>45401</v>
+        <v>45362</v>
       </c>
     </row>
     <row r="58">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>bad customer service</t>
+          <t>constant unwanted calls</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3723,17 +3723,15 @@
           <t>customer service</t>
         </is>
       </c>
-      <c r="E58" t="n">
-        <v>1</v>
-      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>/users/5d0d17c979ad366426e998c9</t>
+          <t>/users/5e2a072261678140a2874591</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>T Hu5541n</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3743,23 +3741,23 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>I became ill over Chrismas</t>
+          <t>I've just had over 20 calls from 118…</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t xml:space="preserve">I became ill over Chrismas, informed these "people" &amp; was granted a two month payment holiday, fine I thought that's sorted. I am now well again they're hounding me to pay "the arrears" &amp; have given me literally days to pay the amount. I called them yesterday to explain my situation but am still getting emails/calls ....5 a day, saying if I don't pay by the end of the month, it's going to impact my credit score &amp; the debt will be sold to a collection agency.Zero compassion companyFollowing this post...I was promised a manager would call me to discuss my account....Still nothing to date 22/4/24 12.22pm. The annoying calls &amp; emails continue. I've just attempted to contact but was placed on hold for 35 minutes, so gave up.Update...the annoying "automated" calls continue despite me clearing my arrears as fast as possible I've managed to speak to a telesales assistant today only to be told "nothing can be done until my arrears are cleared"Still no call from a manager, which I was promised days ago. I was initially pleased by how easy it was to get the loan, I'm now wishing I'd never applied!Terrible company 
+          <t xml:space="preserve">I've just had over 20 calls from 118 118 money non stop over a couple of hours today Friday Afternoon. This is highly suspicious and they will NOT stop ringing me.
 </t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reply from  118 118 MONEY
-Hi Anthony - thank you for coming back to me with your details. I am passing your review to a manager within our Customer Support team. We will be in touch with you shortly.SamCustomer Engagement Team. </t>
+          <t>Reply from  118 118 MONEY
+Hello - I would like to look into this for you - thank you for your review. Please provide some more info to enable us to investigate your complaint.SamCustomer Engagement team.</t>
         </is>
       </c>
       <c r="L58" s="2" t="n">
-        <v>45400</v>
+        <v>45401</v>
       </c>
     </row>
     <row r="59">
@@ -3773,7 +3771,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>unhelpful support and treatment</t>
+          <t>company lacking compassion and following through on promises</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3786,12 +3784,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>/users/5fdd1ca8c14b7e001bcb4acc</t>
+          <t>/users/5d0d17c979ad366426e998c9</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Alison Bage</t>
+          <t>Anthony</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3801,19 +3799,19 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Daily bombardment of texts / emails / calls if you miss a payment!</t>
+          <t>I became ill over Chrismas</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t xml:space="preserve">First of all, I cannot believe that this company has such an excellent rating, I am inclined to believe that they are removing negative reviews as they are probably the worst company I have ever had to deal with when you are needing support.I found myself unexpectedly out of work following a bereavement and therefore in a pickle with money.They initially gave me a short term payment plan after a lot of correspondence. However, once that short term plan was over they have bombarded me with daily calls / texts and emails despite my explaining to them I was under the care of my GP for low mood. They have ignored my last 6 emails over 10 days and have since issued me with a default notice. They are unhelpful with regards to working with you. I made a payment online and they have kept hold of the card details and are using that to make my next contractual payment despite my explaining my expenditure far outweighs my income and I cannot meet those payments. They are underhand and unhelpful with zero compassion and understanding. Be aware of this if you are looking for a loan, go elsewhere if you can. 
+          <t xml:space="preserve">I became ill over Chrismas, informed these "people" &amp; was granted a two month payment holiday, fine I thought that's sorted. I am now well again they're hounding me to pay "the arrears" &amp; have given me literally days to pay the amount. I called them yesterday to explain my situation but am still getting emails/calls ....5 a day, saying if I don't pay by the end of the month, it's going to impact my credit score &amp; the debt will be sold to a collection agency.Zero compassion companyFollowing this post...I was promised a manager would call me to discuss my account....Still nothing to date 22/4/24 12.22pm. The annoying calls &amp; emails continue. I've just attempted to contact but was placed on hold for 35 minutes, so gave up.Update...the annoying "automated" calls continue despite me clearing my arrears as fast as possible I've managed to speak to a telesales assistant today only to be told "nothing can be done until my arrears are cleared"Still no call from a manager, which I was promised days ago. I was initially pleased by how easy it was to get the loan, I'm now wishing I'd never applied!Terrible company 
 </t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Reply from  118 118 MONEY
-Hi Aliso - thank you for your review and for replying to confirm your details. We take this feedback seriously and I'm going to look into this for you. We will come back to you.Kind regardsSamCustomer Engagement Team</t>
+          <t xml:space="preserve">Reply from  118 118 MONEY
+Hi Anthony - thank you for coming back to me with your details. I am passing your review to a manager within our Customer Support team. We will be in touch with you shortly.SamCustomer Engagement Team. </t>
         </is>
       </c>
       <c r="L59" s="2" t="n">
@@ -3831,7 +3829,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>treatment during illness and payment holiday</t>
+          <t>unhelpful support despite difficulties</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3844,12 +3842,12 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>/users/6608266ed315f20012e25990</t>
+          <t>/users/5fdd1ca8c14b7e001bcb4acc</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Michael Perrett</t>
+          <t>Alison Bage</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3859,23 +3857,23 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>Worst card ever</t>
+          <t>Daily bombardment of texts / emails / calls if you miss a payment!</t>
         </is>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Worst card ever, I have a few credit cards and all but 118 have offered me a 3 month payment holiday, when I was struck with illness. These people offered a 30day break having to pay before I was paid from work disgusting way of treating people. And today even though I have not missed a payment but left this honest review they have blocked my card just out of spite, people steer clear of vile lenders like this. 
+          <t xml:space="preserve">First of all, I cannot believe that this company has such an excellent rating, I am inclined to believe that they are removing negative reviews as they are probably the worst company I have ever had to deal with when you are needing support.I found myself unexpectedly out of work following a bereavement and therefore in a pickle with money.They initially gave me a short term payment plan after a lot of correspondence. However, once that short term plan was over they have bombarded me with daily calls / texts and emails despite my explaining to them I was under the care of my GP for low mood. They have ignored my last 6 emails over 10 days and have since issued me with a default notice. They are unhelpful with regards to working with you. I made a payment online and they have kept hold of the card details and are using that to make my next contractual payment despite my explaining my expenditure far outweighs my income and I cannot meet those payments. They are underhand and unhelpful with zero compassion and understanding. Be aware of this if you are looking for a loan, go elsewhere if you can. 
 </t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hello Michael - I'm sorry to hear you're not happy. I have sent a request for you to provide more info, so that I can look into this for you.Your card has not been blocked as a result of leaving a review. If you can respond to our request, we'll happily look into this and come back to you.Sam Customer Engagement Team.</t>
+Hi Aliso - thank you for your review and for replying to confirm your details. We take this feedback seriously and I'm going to look into this for you. We will come back to you.Kind regardsSamCustomer Engagement Team</t>
         </is>
       </c>
       <c r="L60" s="2" t="n">
-        <v>45399</v>
+        <v>45400</v>
       </c>
     </row>
     <row r="61">
@@ -3889,7 +3887,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>long waiting time for support</t>
+          <t>disgusting way of treating people</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -3898,16 +3896,16 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>/users/56f1869f0000ff000a10ee20</t>
+          <t>/users/6608266ed315f20012e25990</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Donna Whitehead</t>
+          <t>Michael Perrett</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3917,18 +3915,23 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>Still not received my card</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr"/>
+          <t>Worst card ever</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Worst card ever, I have a few credit cards and all but 118 have offered me a 3 month payment holiday, when I was struck with illness. These people offered a 30day break having to pay before I was paid from work disgusting way of treating people. And today even though I have not missed a payment but left this honest review they have blocked my card just out of spite, people steer clear of vile lenders like this. 
+</t>
+        </is>
+      </c>
       <c r="K61" t="inlineStr">
         <is>
           <t>Reply from  118 118 MONEY
-Hi Donna - I can see that you posted this review seven days after your application was approved. Please note that we advise it can take up to ten days to receive your card. If you have still not received your card, please call us on 02920 548 118 and we will investigate this for you. SamCustomer Engagement team</t>
+Hello Michael - I'm sorry to hear you're not happy. I have sent a request for you to provide more info, so that I can look into this for you.Your card has not been blocked as a result of leaving a review. If you can respond to our request, we'll happily look into this and come back to you.Sam Customer Engagement Team.</t>
         </is>
       </c>
       <c r="L61" s="2" t="n">
-        <v>45391</v>
+        <v>45399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>